<commit_message>
Pequenas mudanças no código para facilitação ao usuário
</commit_message>
<xml_diff>
--- a/GitHub_análise_v1.xlsx
+++ b/GitHub_análise_v1.xlsx
@@ -115,8 +115,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
     </font>
@@ -141,8 +147,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -165,13 +172,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>